<commit_message>
Inicio da análise macroscópica
</commit_message>
<xml_diff>
--- a/data/etapa_2/Análise Metais.xlsx
+++ b/data/etapa_2/Análise Metais.xlsx
@@ -329,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -384,6 +384,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="8" fillId="7" fontId="4" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
@@ -442,10 +445,16 @@
     <xf borderId="8" fillId="24" fontId="4" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -843,14 +852,32 @@
       <c r="I6" s="16">
         <v>0.2978</v>
       </c>
+      <c r="J6" s="21">
+        <v>0.0259</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0.1917</v>
+      </c>
+      <c r="L6" s="16">
+        <v>-0.1347</v>
+      </c>
+      <c r="M6" s="21">
+        <v>0.0215</v>
+      </c>
+      <c r="N6" s="21">
+        <v>0.0688</v>
+      </c>
+      <c r="O6" s="21">
+        <v>0.2917</v>
+      </c>
       <c r="P6" s="17">
         <f t="shared" si="1"/>
-        <v>0.2978</v>
+        <v>0.0061</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="18"/>
-      <c r="C7" s="21">
+      <c r="C7" s="22">
         <v>50.0</v>
       </c>
       <c r="D7" s="16">
@@ -871,14 +898,32 @@
       <c r="I7" s="16">
         <v>0.3529</v>
       </c>
+      <c r="J7" s="21">
+        <v>0.0285</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0.2389</v>
+      </c>
+      <c r="L7" s="16">
+        <v>-0.1273</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0.0689</v>
+      </c>
+      <c r="N7" s="21">
+        <v>0.1149</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0.4578</v>
+      </c>
       <c r="P7" s="17">
         <f t="shared" si="1"/>
-        <v>0.3529</v>
+        <v>-0.1049</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="18"/>
-      <c r="C8" s="22">
+      <c r="C8" s="23">
         <v>75.0</v>
       </c>
       <c r="D8" s="16">
@@ -899,14 +944,32 @@
       <c r="I8" s="16">
         <v>0.4787</v>
       </c>
+      <c r="J8" s="21">
+        <v>0.0298</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0.3031</v>
+      </c>
+      <c r="L8" s="16">
+        <v>-0.1202</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0.0267</v>
+      </c>
+      <c r="N8" s="21">
+        <v>0.0782</v>
+      </c>
+      <c r="O8" s="21">
+        <v>0.978</v>
+      </c>
       <c r="P8" s="17">
         <f t="shared" si="1"/>
-        <v>0.4787</v>
+        <v>-0.4993</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="9"/>
-      <c r="C9" s="23">
+      <c r="C9" s="24">
         <v>100.0</v>
       </c>
       <c r="D9" s="16">
@@ -927,16 +990,34 @@
       <c r="I9" s="16">
         <v>0.8855</v>
       </c>
+      <c r="J9" s="21">
+        <v>0.0276</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0.322</v>
+      </c>
+      <c r="L9" s="16">
+        <v>-0.1166</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0.0169</v>
+      </c>
+      <c r="N9" s="21">
+        <v>0.0388</v>
+      </c>
+      <c r="O9" s="21">
+        <v>0.9658</v>
+      </c>
       <c r="P9" s="17">
         <f t="shared" si="1"/>
-        <v>0.8855</v>
+        <v>-0.0803</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="26">
         <v>0.0</v>
       </c>
       <c r="D10" s="16">
@@ -955,6 +1036,24 @@
         <v>0.0</v>
       </c>
       <c r="I10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O10" s="16">
         <v>0.0</v>
       </c>
       <c r="P10" s="17">
@@ -964,7 +1063,7 @@
     </row>
     <row r="11">
       <c r="B11" s="18"/>
-      <c r="C11" s="26">
+      <c r="C11" s="27">
         <v>25.0</v>
       </c>
       <c r="D11" s="16">
@@ -985,14 +1084,32 @@
       <c r="I11" s="16">
         <v>0.2978</v>
       </c>
+      <c r="J11" s="21">
+        <v>0.0274</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0.1992</v>
+      </c>
+      <c r="L11" s="16">
+        <v>-0.1347</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0.023</v>
+      </c>
+      <c r="N11" s="21">
+        <v>0.1043</v>
+      </c>
+      <c r="O11" s="21">
+        <v>0.3213</v>
+      </c>
       <c r="P11" s="17">
         <f t="shared" si="1"/>
-        <v>0.2978</v>
+        <v>-0.0235</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="18"/>
-      <c r="C12" s="27">
+      <c r="C12" s="28">
         <v>50.0</v>
       </c>
       <c r="D12" s="16">
@@ -1013,14 +1130,32 @@
       <c r="I12" s="16">
         <v>0.3529</v>
       </c>
+      <c r="J12" s="21">
+        <v>0.0316</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0.2352</v>
+      </c>
+      <c r="L12" s="16">
+        <v>-0.1273</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0.005</v>
+      </c>
+      <c r="N12" s="21">
+        <v>0.0485</v>
+      </c>
+      <c r="O12" s="21">
+        <v>0.68</v>
+      </c>
       <c r="P12" s="17">
         <f t="shared" si="1"/>
-        <v>0.3529</v>
+        <v>-0.3271</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="18"/>
-      <c r="C13" s="28">
+      <c r="C13" s="29">
         <v>75.0</v>
       </c>
       <c r="D13" s="16">
@@ -1041,14 +1176,32 @@
       <c r="I13" s="16">
         <v>0.4787</v>
       </c>
+      <c r="J13" s="21">
+        <v>0.0339</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0.2811</v>
+      </c>
+      <c r="L13" s="16">
+        <v>-0.1202</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0.0098</v>
+      </c>
+      <c r="N13" s="21">
+        <v>0.0855</v>
+      </c>
+      <c r="O13" s="21">
+        <v>0.5591</v>
+      </c>
       <c r="P13" s="17">
         <f t="shared" si="1"/>
-        <v>0.4787</v>
+        <v>-0.0804</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="9"/>
-      <c r="C14" s="29">
+      <c r="C14" s="30">
         <v>100.0</v>
       </c>
       <c r="D14" s="16">
@@ -1069,16 +1222,34 @@
       <c r="I14" s="16">
         <v>0.8855</v>
       </c>
+      <c r="J14" s="21">
+        <v>0.0332</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0.3274</v>
+      </c>
+      <c r="L14" s="16">
+        <v>-0.1166</v>
+      </c>
+      <c r="M14" s="21">
+        <v>0.1676</v>
+      </c>
+      <c r="N14" s="21">
+        <v>0.0603</v>
+      </c>
+      <c r="O14" s="21">
+        <v>0.3886</v>
+      </c>
       <c r="P14" s="17">
         <f t="shared" si="1"/>
-        <v>0.8855</v>
+        <v>0.4969</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="31">
         <v>0.0</v>
       </c>
       <c r="D15" s="16">
@@ -1097,6 +1268,24 @@
         <v>0.0</v>
       </c>
       <c r="I15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="K15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O15" s="16">
         <v>0.0</v>
       </c>
       <c r="P15" s="17">
@@ -1106,7 +1295,7 @@
     </row>
     <row r="16">
       <c r="B16" s="18"/>
-      <c r="C16" s="31">
+      <c r="C16" s="32">
         <v>25.0</v>
       </c>
       <c r="D16" s="16">
@@ -1127,14 +1316,32 @@
       <c r="I16" s="16">
         <v>0.2433</v>
       </c>
+      <c r="J16" s="21">
+        <v>0.0345</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0.203</v>
+      </c>
+      <c r="L16" s="16">
+        <v>-0.1376</v>
+      </c>
+      <c r="M16" s="21">
+        <v>0.0467</v>
+      </c>
+      <c r="N16" s="21">
+        <v>0.1281</v>
+      </c>
+      <c r="O16" s="21">
+        <v>0.4179</v>
+      </c>
       <c r="P16" s="17">
         <f t="shared" si="1"/>
-        <v>0.2433</v>
+        <v>-0.1746</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="18"/>
-      <c r="C17" s="32">
+      <c r="C17" s="33">
         <v>50.0</v>
       </c>
       <c r="D17" s="16">
@@ -1155,14 +1362,32 @@
       <c r="I17" s="16">
         <v>0.2913</v>
       </c>
+      <c r="J17" s="21">
+        <v>0.038</v>
+      </c>
+      <c r="K17" s="21">
+        <v>0.2408</v>
+      </c>
+      <c r="L17" s="16">
+        <v>-0.1242</v>
+      </c>
+      <c r="M17" s="21">
+        <v>0.0885</v>
+      </c>
+      <c r="N17" s="21">
+        <v>0.0374</v>
+      </c>
+      <c r="O17" s="21">
+        <v>0.6306</v>
+      </c>
       <c r="P17" s="17">
         <f t="shared" si="1"/>
-        <v>0.2913</v>
+        <v>-0.3393</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="18"/>
-      <c r="C18" s="33">
+      <c r="C18" s="34">
         <v>75.0</v>
       </c>
       <c r="D18" s="16">
@@ -1183,14 +1408,32 @@
       <c r="I18" s="16">
         <v>0.4162</v>
       </c>
+      <c r="J18" s="21">
+        <v>0.0336</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0.2741</v>
+      </c>
+      <c r="L18" s="16">
+        <v>-0.1205</v>
+      </c>
+      <c r="M18" s="21">
+        <v>0.1463</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0.0399</v>
+      </c>
+      <c r="O18" s="21">
+        <v>0.3521</v>
+      </c>
       <c r="P18" s="17">
         <f t="shared" si="1"/>
-        <v>0.4162</v>
+        <v>0.0641</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="9"/>
-      <c r="C19" s="34">
+      <c r="C19" s="35">
         <v>100.0</v>
       </c>
       <c r="D19" s="16">
@@ -1211,16 +1454,34 @@
       <c r="I19" s="16">
         <v>0.7157</v>
       </c>
+      <c r="J19" s="21">
+        <v>0.0365</v>
+      </c>
+      <c r="K19" s="21">
+        <v>0.3092</v>
+      </c>
+      <c r="L19" s="16">
+        <v>-0.1124</v>
+      </c>
+      <c r="M19" s="21">
+        <v>0.1753</v>
+      </c>
+      <c r="N19" s="21">
+        <v>0.0862</v>
+      </c>
+      <c r="O19" s="21">
+        <v>0.4127</v>
+      </c>
       <c r="P19" s="17">
         <f t="shared" si="1"/>
-        <v>0.7157</v>
+        <v>0.303</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="36">
         <v>0.0</v>
       </c>
       <c r="D20" s="16">
@@ -1239,6 +1500,24 @@
         <v>0.0</v>
       </c>
       <c r="I20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="J20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O20" s="16">
         <v>0.0</v>
       </c>
       <c r="P20" s="17">
@@ -1248,7 +1527,7 @@
     </row>
     <row r="21">
       <c r="B21" s="18"/>
-      <c r="C21" s="36">
+      <c r="C21" s="37">
         <v>25.0</v>
       </c>
       <c r="D21" s="16">
@@ -1269,14 +1548,32 @@
       <c r="I21" s="16">
         <v>0.2433</v>
       </c>
+      <c r="J21" s="21">
+        <v>0.033</v>
+      </c>
+      <c r="K21" s="21">
+        <v>0.2042</v>
+      </c>
+      <c r="L21" s="16">
+        <v>-0.1376</v>
+      </c>
+      <c r="M21" s="21">
+        <v>0.0458</v>
+      </c>
+      <c r="N21" s="21">
+        <v>0.0748</v>
+      </c>
+      <c r="O21" s="21">
+        <v>0.4085</v>
+      </c>
       <c r="P21" s="17">
         <f t="shared" si="1"/>
-        <v>0.2433</v>
+        <v>-0.1652</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="18"/>
-      <c r="C22" s="37">
+      <c r="C22" s="38">
         <v>50.0</v>
       </c>
       <c r="D22" s="16">
@@ -1297,14 +1594,32 @@
       <c r="I22" s="16">
         <v>0.2913</v>
       </c>
+      <c r="J22" s="21">
+        <v>0.0349</v>
+      </c>
+      <c r="K22" s="21">
+        <v>0.2497</v>
+      </c>
+      <c r="L22" s="20">
+        <v>-0.1242</v>
+      </c>
+      <c r="M22" s="21">
+        <v>0.075</v>
+      </c>
+      <c r="N22" s="21">
+        <v>0.0895</v>
+      </c>
+      <c r="O22" s="21">
+        <v>0.5847</v>
+      </c>
       <c r="P22" s="17">
         <f t="shared" si="1"/>
-        <v>0.2913</v>
+        <v>-0.2934</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="18"/>
-      <c r="C23" s="38">
+      <c r="C23" s="39">
         <v>75.0</v>
       </c>
       <c r="D23" s="16">
@@ -1325,14 +1640,32 @@
       <c r="I23" s="16">
         <v>0.4162</v>
       </c>
+      <c r="J23" s="21">
+        <v>0.033</v>
+      </c>
+      <c r="K23" s="21">
+        <v>0.2822</v>
+      </c>
+      <c r="L23" s="20">
+        <v>-0.1205</v>
+      </c>
+      <c r="M23" s="21">
+        <v>0.1384</v>
+      </c>
+      <c r="N23" s="21">
+        <v>0.0887</v>
+      </c>
+      <c r="O23" s="21">
+        <v>0.3811</v>
+      </c>
       <c r="P23" s="17">
         <f t="shared" si="1"/>
-        <v>0.4162</v>
+        <v>0.0351</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="9"/>
-      <c r="C24" s="39">
+      <c r="C24" s="40">
         <v>100.0</v>
       </c>
       <c r="D24" s="16">
@@ -1353,9 +1686,27 @@
       <c r="I24" s="16">
         <v>0.7157</v>
       </c>
+      <c r="J24" s="21">
+        <v>0.0362</v>
+      </c>
+      <c r="K24" s="21">
+        <v>0.3209</v>
+      </c>
+      <c r="L24" s="20">
+        <v>-0.1124</v>
+      </c>
+      <c r="M24" s="21">
+        <v>0.1692</v>
+      </c>
+      <c r="N24" s="21">
+        <v>0.098</v>
+      </c>
+      <c r="O24" s="21">
+        <v>0.3919</v>
+      </c>
       <c r="P24" s="17">
         <f t="shared" si="1"/>
-        <v>0.7157</v>
+        <v>0.3238</v>
       </c>
     </row>
     <row r="25">
@@ -4380,7 +4731,7 @@
       <c r="I5" s="16">
         <v>0.0</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="41">
         <v>0.0</v>
       </c>
       <c r="K5" s="16">
@@ -4426,14 +4777,32 @@
       <c r="I6" s="16">
         <v>0.7161</v>
       </c>
+      <c r="J6" s="42">
+        <v>0.0087</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0.1883</v>
+      </c>
+      <c r="L6" s="16">
+        <v>-0.1151</v>
+      </c>
+      <c r="M6" s="21">
+        <v>0.0266</v>
+      </c>
+      <c r="N6" s="21">
+        <v>0.0643</v>
+      </c>
+      <c r="O6" s="21">
+        <v>0.5287</v>
+      </c>
       <c r="P6" s="17">
         <f t="shared" si="1"/>
-        <v>0.7161</v>
+        <v>0.1874</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="18"/>
-      <c r="C7" s="21">
+      <c r="C7" s="22">
         <v>50.0</v>
       </c>
       <c r="D7" s="20">
@@ -4454,14 +4823,32 @@
       <c r="I7" s="16">
         <v>2.0249</v>
       </c>
+      <c r="J7" s="42">
+        <v>0.0036</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0.2173</v>
+      </c>
+      <c r="L7" s="16">
+        <v>-0.1029</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0.0492</v>
+      </c>
+      <c r="N7" s="21">
+        <v>0.0688</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0.8279</v>
+      </c>
       <c r="P7" s="17">
         <f t="shared" si="1"/>
-        <v>2.0249</v>
+        <v>1.197</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="18"/>
-      <c r="C8" s="22">
+      <c r="C8" s="23">
         <v>75.0</v>
       </c>
       <c r="D8" s="20">
@@ -4482,14 +4869,32 @@
       <c r="I8" s="16">
         <v>1.0198</v>
       </c>
+      <c r="J8" s="42">
+        <v>0.005</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0.2495</v>
+      </c>
+      <c r="L8" s="16">
+        <v>-0.0971</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0.0631</v>
+      </c>
+      <c r="N8" s="21">
+        <v>0.054</v>
+      </c>
+      <c r="O8" s="21">
+        <v>0.5335</v>
+      </c>
       <c r="P8" s="17">
         <f t="shared" si="1"/>
-        <v>1.0198</v>
+        <v>0.4863</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="9"/>
-      <c r="C9" s="23">
+      <c r="C9" s="24">
         <v>100.0</v>
       </c>
       <c r="D9" s="20">
@@ -4510,16 +4915,34 @@
       <c r="I9" s="16">
         <v>1.6505</v>
       </c>
+      <c r="J9" s="42">
+        <v>0.0054</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0.2543</v>
+      </c>
+      <c r="L9" s="16">
+        <v>-0.0956</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0.0896</v>
+      </c>
+      <c r="N9" s="21">
+        <v>0.0527</v>
+      </c>
+      <c r="O9" s="21">
+        <v>0.4732</v>
+      </c>
       <c r="P9" s="17">
         <f t="shared" si="1"/>
-        <v>1.6505</v>
+        <v>1.1773</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="26">
         <v>0.0</v>
       </c>
       <c r="D10" s="16">
@@ -4538,6 +4961,24 @@
         <v>0.0</v>
       </c>
       <c r="I10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="41">
+        <v>0.0</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O10" s="16">
         <v>0.0</v>
       </c>
       <c r="P10" s="17">
@@ -4547,7 +4988,7 @@
     </row>
     <row r="11">
       <c r="B11" s="18"/>
-      <c r="C11" s="26">
+      <c r="C11" s="27">
         <v>25.0</v>
       </c>
       <c r="D11" s="20">
@@ -4568,14 +5009,32 @@
       <c r="I11" s="16">
         <v>0.7161</v>
       </c>
+      <c r="J11" s="43">
+        <v>0.0099</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0.1094</v>
+      </c>
+      <c r="L11" s="16">
+        <v>-0.1151</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0.0227</v>
+      </c>
+      <c r="N11" s="21">
+        <v>0.0162</v>
+      </c>
+      <c r="O11" s="21">
+        <v>0.266</v>
+      </c>
       <c r="P11" s="17">
         <f t="shared" si="1"/>
-        <v>0.7161</v>
+        <v>0.4501</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="18"/>
-      <c r="C12" s="27">
+      <c r="C12" s="28">
         <v>50.0</v>
       </c>
       <c r="D12" s="20">
@@ -4596,14 +5055,32 @@
       <c r="I12" s="16">
         <v>2.0249</v>
       </c>
+      <c r="J12" s="43">
+        <v>0.0097</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0.2212</v>
+      </c>
+      <c r="L12" s="16">
+        <v>-0.1029</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0.0452</v>
+      </c>
+      <c r="N12" s="21">
+        <v>0.0312</v>
+      </c>
+      <c r="O12" s="21">
+        <v>0.7778</v>
+      </c>
       <c r="P12" s="17">
         <f t="shared" si="1"/>
-        <v>2.0249</v>
+        <v>1.2471</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="18"/>
-      <c r="C13" s="28">
+      <c r="C13" s="29">
         <v>75.0</v>
       </c>
       <c r="D13" s="20">
@@ -4624,14 +5101,32 @@
       <c r="I13" s="16">
         <v>1.0198</v>
       </c>
+      <c r="J13" s="42">
+        <v>0.0078</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0.2394</v>
+      </c>
+      <c r="L13" s="16">
+        <v>-0.0971</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0.0642</v>
+      </c>
+      <c r="N13" s="21">
+        <v>0.059</v>
+      </c>
+      <c r="O13" s="21">
+        <v>0.279</v>
+      </c>
       <c r="P13" s="17">
         <f t="shared" si="1"/>
-        <v>1.0198</v>
+        <v>0.7408</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="9"/>
-      <c r="C14" s="29">
+      <c r="C14" s="30">
         <v>100.0</v>
       </c>
       <c r="D14" s="20">
@@ -4652,16 +5147,34 @@
       <c r="I14" s="16">
         <v>1.6505</v>
       </c>
+      <c r="J14" s="42">
+        <v>0.0107</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0.2742</v>
+      </c>
+      <c r="L14" s="16">
+        <v>-0.0956</v>
+      </c>
+      <c r="M14" s="21">
+        <v>0.0761</v>
+      </c>
+      <c r="N14" s="21">
+        <v>0.0243</v>
+      </c>
+      <c r="O14" s="21">
+        <v>1.0763</v>
+      </c>
       <c r="P14" s="17">
         <f t="shared" si="1"/>
-        <v>1.6505</v>
+        <v>0.5742</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="31">
         <v>0.0</v>
       </c>
       <c r="D15" s="16">
@@ -4680,6 +5193,24 @@
         <v>0.0</v>
       </c>
       <c r="I15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="41">
+        <v>0.0</v>
+      </c>
+      <c r="K15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O15" s="16">
         <v>0.0</v>
       </c>
       <c r="P15" s="17">
@@ -4689,7 +5220,7 @@
     </row>
     <row r="16">
       <c r="B16" s="18"/>
-      <c r="C16" s="31">
+      <c r="C16" s="32">
         <v>25.0</v>
       </c>
       <c r="D16" s="20">
@@ -4710,14 +5241,32 @@
       <c r="I16" s="16">
         <v>0.6219</v>
       </c>
+      <c r="J16" s="42">
+        <v>0.011</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0.1884</v>
+      </c>
+      <c r="L16" s="16">
+        <v>-0.1053</v>
+      </c>
+      <c r="M16" s="21">
+        <v>0.0124</v>
+      </c>
+      <c r="N16" s="21">
+        <v>0.0387</v>
+      </c>
+      <c r="O16" s="21">
+        <v>0.2855</v>
+      </c>
       <c r="P16" s="17">
         <f t="shared" si="1"/>
-        <v>0.6219</v>
+        <v>0.3364</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="18"/>
-      <c r="C17" s="32">
+      <c r="C17" s="33">
         <v>50.0</v>
       </c>
       <c r="D17" s="20">
@@ -4738,14 +5287,32 @@
       <c r="I17" s="16">
         <v>0.688</v>
       </c>
+      <c r="J17" s="42">
+        <v>0.0117</v>
+      </c>
+      <c r="K17" s="21">
+        <v>0.225</v>
+      </c>
+      <c r="L17" s="16">
+        <v>-0.1167</v>
+      </c>
+      <c r="M17" s="21">
+        <v>0.0336</v>
+      </c>
+      <c r="N17" s="21">
+        <v>0.0772</v>
+      </c>
+      <c r="O17" s="21">
+        <v>0.9342</v>
+      </c>
       <c r="P17" s="17">
         <f t="shared" si="1"/>
-        <v>0.688</v>
+        <v>-0.2462</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="18"/>
-      <c r="C18" s="33">
+      <c r="C18" s="34">
         <v>75.0</v>
       </c>
       <c r="D18" s="20">
@@ -4766,14 +5333,32 @@
       <c r="I18" s="16">
         <v>0.8298</v>
       </c>
+      <c r="J18" s="42">
+        <v>0.0127</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0.2589</v>
+      </c>
+      <c r="L18" s="16">
+        <v>-0.1134</v>
+      </c>
+      <c r="M18" s="21">
+        <v>0.0488</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0.0163</v>
+      </c>
+      <c r="O18" s="21">
+        <v>0.5304</v>
+      </c>
       <c r="P18" s="17">
         <f t="shared" si="1"/>
-        <v>0.8298</v>
+        <v>0.2994</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="9"/>
-      <c r="C19" s="34">
+      <c r="C19" s="35">
         <v>100.0</v>
       </c>
       <c r="D19" s="20">
@@ -4794,16 +5379,34 @@
       <c r="I19" s="16">
         <v>0.7797</v>
       </c>
+      <c r="J19" s="42">
+        <v>0.0123</v>
+      </c>
+      <c r="K19" s="21">
+        <v>0.285</v>
+      </c>
+      <c r="L19" s="16">
+        <v>0.1109</v>
+      </c>
+      <c r="M19" s="21">
+        <v>0.0522</v>
+      </c>
+      <c r="N19" s="21">
+        <v>0.0685</v>
+      </c>
+      <c r="O19" s="21">
+        <v>0.7639</v>
+      </c>
       <c r="P19" s="17">
         <f t="shared" si="1"/>
-        <v>0.7797</v>
+        <v>0.0158</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="36">
         <v>0.0</v>
       </c>
       <c r="D20" s="16">
@@ -4822,6 +5425,24 @@
         <v>0.0</v>
       </c>
       <c r="I20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="J20" s="41">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O20" s="16">
         <v>0.0</v>
       </c>
       <c r="P20" s="17">
@@ -4831,7 +5452,7 @@
     </row>
     <row r="21">
       <c r="B21" s="18"/>
-      <c r="C21" s="36">
+      <c r="C21" s="37">
         <v>25.0</v>
       </c>
       <c r="D21" s="20">
@@ -4852,14 +5473,32 @@
       <c r="I21" s="16">
         <v>0.6219</v>
       </c>
+      <c r="J21" s="42">
+        <v>0.0111</v>
+      </c>
+      <c r="K21" s="21">
+        <v>0.1929</v>
+      </c>
+      <c r="L21" s="16">
+        <v>-0.1053</v>
+      </c>
+      <c r="M21" s="21">
+        <v>0.0105</v>
+      </c>
+      <c r="N21" s="21">
+        <v>0.0427</v>
+      </c>
+      <c r="O21" s="21">
+        <v>0.4253</v>
+      </c>
       <c r="P21" s="17">
         <f t="shared" si="1"/>
-        <v>0.6219</v>
+        <v>0.1966</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="18"/>
-      <c r="C22" s="37">
+      <c r="C22" s="38">
         <v>50.0</v>
       </c>
       <c r="D22" s="20">
@@ -4880,14 +5519,32 @@
       <c r="I22" s="16">
         <v>0.688</v>
       </c>
+      <c r="J22" s="42">
+        <v>0.0131</v>
+      </c>
+      <c r="K22" s="21">
+        <v>0.2256</v>
+      </c>
+      <c r="L22" s="16">
+        <v>-0.1167</v>
+      </c>
+      <c r="M22" s="21">
+        <v>0.037</v>
+      </c>
+      <c r="N22" s="21">
+        <v>0.0517</v>
+      </c>
+      <c r="O22" s="21">
+        <v>0.6759</v>
+      </c>
       <c r="P22" s="17">
         <f t="shared" si="1"/>
-        <v>0.688</v>
+        <v>0.0121</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="18"/>
-      <c r="C23" s="38">
+      <c r="C23" s="39">
         <v>75.0</v>
       </c>
       <c r="D23" s="20">
@@ -4908,14 +5565,32 @@
       <c r="I23" s="16">
         <v>0.8298</v>
       </c>
+      <c r="J23" s="42">
+        <v>0.0182</v>
+      </c>
+      <c r="K23" s="21">
+        <v>0.2562</v>
+      </c>
+      <c r="L23" s="16">
+        <v>-0.1134</v>
+      </c>
+      <c r="M23" s="21">
+        <v>0.0546</v>
+      </c>
+      <c r="N23" s="21">
+        <v>0.0569</v>
+      </c>
+      <c r="O23" s="21">
+        <v>0.3209</v>
+      </c>
       <c r="P23" s="17">
         <f t="shared" si="1"/>
-        <v>0.8298</v>
+        <v>0.5089</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="9"/>
-      <c r="C24" s="39">
+      <c r="C24" s="40">
         <v>100.0</v>
       </c>
       <c r="D24" s="20">
@@ -4936,9 +5611,27 @@
       <c r="I24" s="16">
         <v>0.7797</v>
       </c>
+      <c r="J24" s="42">
+        <v>0.015</v>
+      </c>
+      <c r="K24" s="21">
+        <v>0.2696</v>
+      </c>
+      <c r="L24" s="16">
+        <v>0.1109</v>
+      </c>
+      <c r="M24" s="21">
+        <v>0.0204</v>
+      </c>
+      <c r="N24" s="21">
+        <v>0.0275</v>
+      </c>
+      <c r="O24" s="21">
+        <v>0.3193</v>
+      </c>
       <c r="P24" s="17">
         <f t="shared" si="1"/>
-        <v>0.7797</v>
+        <v>0.4604</v>
       </c>
     </row>
     <row r="25">
@@ -7966,10 +8659,10 @@
       <c r="J5" s="16">
         <v>0.0</v>
       </c>
-      <c r="K5" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="L5" s="40">
+      <c r="K5" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L5" s="44">
         <v>0.0</v>
       </c>
       <c r="M5" s="16">
@@ -8009,22 +8702,22 @@
       <c r="I6" s="16">
         <v>0.2978</v>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="44">
         <v>-0.0066</v>
       </c>
-      <c r="K6" s="40">
+      <c r="K6" s="44">
         <v>0.2034</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="21">
         <v>-0.0196</v>
       </c>
       <c r="M6" s="16">
         <v>0.1513</v>
       </c>
-      <c r="N6" s="40">
+      <c r="N6" s="44">
         <v>0.1455</v>
       </c>
-      <c r="O6" s="40">
+      <c r="O6" s="44">
         <v>0.1232</v>
       </c>
       <c r="P6" s="17">
@@ -8034,7 +8727,7 @@
     </row>
     <row r="7">
       <c r="B7" s="18"/>
-      <c r="C7" s="21">
+      <c r="C7" s="22">
         <v>50.0</v>
       </c>
       <c r="D7" s="16">
@@ -8055,22 +8748,22 @@
       <c r="I7" s="16">
         <v>0.3529</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="44">
         <v>-0.0031</v>
       </c>
-      <c r="K7" s="40">
+      <c r="K7" s="44">
         <v>0.3299</v>
       </c>
-      <c r="L7" s="41">
+      <c r="L7" s="21">
         <v>-0.0297</v>
       </c>
       <c r="M7" s="16">
         <v>0.2029</v>
       </c>
-      <c r="N7" s="40">
+      <c r="N7" s="44">
         <v>0.1813</v>
       </c>
-      <c r="O7" s="40">
+      <c r="O7" s="44">
         <v>0.2409</v>
       </c>
       <c r="P7" s="17">
@@ -8080,7 +8773,7 @@
     </row>
     <row r="8">
       <c r="B8" s="18"/>
-      <c r="C8" s="22">
+      <c r="C8" s="23">
         <v>75.0</v>
       </c>
       <c r="D8" s="16">
@@ -8101,22 +8794,22 @@
       <c r="I8" s="16">
         <v>0.4787</v>
       </c>
-      <c r="J8" s="40">
+      <c r="J8" s="44">
         <v>-0.0049</v>
       </c>
-      <c r="K8" s="40">
+      <c r="K8" s="44">
         <v>0.4319</v>
       </c>
-      <c r="L8" s="41">
+      <c r="L8" s="21">
         <v>-0.0396</v>
       </c>
       <c r="M8" s="16">
         <v>0.2647</v>
       </c>
-      <c r="N8" s="40">
+      <c r="N8" s="44">
         <v>0.188</v>
       </c>
-      <c r="O8" s="40">
+      <c r="O8" s="44">
         <v>0.3373</v>
       </c>
       <c r="P8" s="17">
@@ -8126,7 +8819,7 @@
     </row>
     <row r="9">
       <c r="B9" s="9"/>
-      <c r="C9" s="23">
+      <c r="C9" s="24">
         <v>100.0</v>
       </c>
       <c r="D9" s="16">
@@ -8147,22 +8840,22 @@
       <c r="I9" s="16">
         <v>0.8855</v>
       </c>
-      <c r="J9" s="40">
+      <c r="J9" s="44">
         <v>-0.003</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K9" s="44">
         <v>0.5099</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="21">
         <v>-0.0423</v>
       </c>
       <c r="M9" s="16">
         <v>0.3327</v>
       </c>
-      <c r="N9" s="40">
+      <c r="N9" s="44">
         <v>0.217</v>
       </c>
-      <c r="O9" s="40">
+      <c r="O9" s="44">
         <v>0.413</v>
       </c>
       <c r="P9" s="17">
@@ -8171,10 +8864,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="26">
         <v>0.0</v>
       </c>
       <c r="D10" s="16">
@@ -8195,22 +8888,22 @@
       <c r="I10" s="16">
         <v>0.0</v>
       </c>
-      <c r="J10" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="K10" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="L10" s="40">
+      <c r="J10" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="K10" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L10" s="44">
         <v>0.0</v>
       </c>
       <c r="M10" s="16">
         <v>0.0</v>
       </c>
-      <c r="N10" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="O10" s="40">
+      <c r="N10" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="O10" s="44">
         <v>0.0</v>
       </c>
       <c r="P10" s="17">
@@ -8220,7 +8913,7 @@
     </row>
     <row r="11">
       <c r="B11" s="18"/>
-      <c r="C11" s="26">
+      <c r="C11" s="27">
         <v>25.0</v>
       </c>
       <c r="D11" s="16">
@@ -8241,22 +8934,22 @@
       <c r="I11" s="16">
         <v>0.2978</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="44">
         <v>-0.0062</v>
       </c>
-      <c r="K11" s="40">
+      <c r="K11" s="44">
         <v>0.2378</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="21">
         <v>-0.0795</v>
       </c>
       <c r="M11" s="16">
         <v>0.1818</v>
       </c>
-      <c r="N11" s="40">
+      <c r="N11" s="44">
         <v>0.2304</v>
       </c>
-      <c r="O11" s="40">
+      <c r="O11" s="44">
         <v>0.1627</v>
       </c>
       <c r="P11" s="17">
@@ -8266,7 +8959,7 @@
     </row>
     <row r="12">
       <c r="B12" s="18"/>
-      <c r="C12" s="27">
+      <c r="C12" s="28">
         <v>50.0</v>
       </c>
       <c r="D12" s="16">
@@ -8287,22 +8980,22 @@
       <c r="I12" s="16">
         <v>0.3529</v>
       </c>
-      <c r="J12" s="40">
+      <c r="J12" s="44">
         <v>-0.0039</v>
       </c>
-      <c r="K12" s="40">
+      <c r="K12" s="44">
         <v>0.345</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="21">
         <v>-0.0681</v>
       </c>
       <c r="M12" s="16">
         <v>0.2461</v>
       </c>
-      <c r="N12" s="40">
+      <c r="N12" s="44">
         <v>0.2309</v>
       </c>
-      <c r="O12" s="40">
+      <c r="O12" s="44">
         <v>0.2211</v>
       </c>
       <c r="P12" s="17">
@@ -8312,7 +9005,7 @@
     </row>
     <row r="13">
       <c r="B13" s="18"/>
-      <c r="C13" s="28">
+      <c r="C13" s="29">
         <v>75.0</v>
       </c>
       <c r="D13" s="16">
@@ -8333,22 +9026,22 @@
       <c r="I13" s="16">
         <v>0.4787</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="44">
         <v>-0.0029</v>
       </c>
-      <c r="K13" s="40">
+      <c r="K13" s="44">
         <v>0.4166</v>
       </c>
-      <c r="L13" s="41">
+      <c r="L13" s="21">
         <v>-0.0714</v>
       </c>
       <c r="M13" s="16">
         <v>0.3024</v>
       </c>
-      <c r="N13" s="40">
+      <c r="N13" s="44">
         <v>0.2551</v>
       </c>
-      <c r="O13" s="40">
+      <c r="O13" s="44">
         <v>0.3102</v>
       </c>
       <c r="P13" s="17">
@@ -8358,7 +9051,7 @@
     </row>
     <row r="14">
       <c r="B14" s="9"/>
-      <c r="C14" s="29">
+      <c r="C14" s="30">
         <v>100.0</v>
       </c>
       <c r="D14" s="16">
@@ -8379,22 +9072,22 @@
       <c r="I14" s="16">
         <v>0.8855</v>
       </c>
-      <c r="J14" s="40">
+      <c r="J14" s="44">
         <v>-0.004</v>
       </c>
-      <c r="K14" s="40">
+      <c r="K14" s="44">
         <v>0.4904</v>
       </c>
-      <c r="L14" s="41">
+      <c r="L14" s="21">
         <v>-0.0797</v>
       </c>
       <c r="M14" s="16">
         <v>0.328</v>
       </c>
-      <c r="N14" s="40">
+      <c r="N14" s="44">
         <v>0.2683</v>
       </c>
-      <c r="O14" s="40">
+      <c r="O14" s="44">
         <v>0.3812</v>
       </c>
       <c r="P14" s="17">
@@ -8403,10 +9096,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="31">
         <v>0.0</v>
       </c>
       <c r="D15" s="16">
@@ -8427,22 +9120,22 @@
       <c r="I15" s="16">
         <v>0.0</v>
       </c>
-      <c r="J15" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="K15" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="L15" s="40">
+      <c r="J15" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="K15" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L15" s="44">
         <v>0.0</v>
       </c>
       <c r="M15" s="16">
         <v>0.0</v>
       </c>
-      <c r="N15" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="O15" s="40">
+      <c r="N15" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="O15" s="44">
         <v>0.0</v>
       </c>
       <c r="P15" s="17">
@@ -8452,7 +9145,7 @@
     </row>
     <row r="16">
       <c r="B16" s="18"/>
-      <c r="C16" s="31">
+      <c r="C16" s="32">
         <v>25.0</v>
       </c>
       <c r="D16" s="16">
@@ -8473,22 +9166,22 @@
       <c r="I16" s="16">
         <v>0.2433</v>
       </c>
-      <c r="J16" s="40">
+      <c r="J16" s="44">
         <v>-0.0015</v>
       </c>
-      <c r="K16" s="40">
+      <c r="K16" s="44">
         <v>0.2491</v>
       </c>
-      <c r="L16" s="41">
+      <c r="L16" s="21">
         <v>-0.1017</v>
       </c>
       <c r="M16" s="16">
         <v>0.2379</v>
       </c>
-      <c r="N16" s="40">
+      <c r="N16" s="44">
         <v>0.2979</v>
       </c>
-      <c r="O16" s="40">
+      <c r="O16" s="44">
         <v>0.8145</v>
       </c>
       <c r="P16" s="17">
@@ -8498,7 +9191,7 @@
     </row>
     <row r="17">
       <c r="B17" s="18"/>
-      <c r="C17" s="32">
+      <c r="C17" s="33">
         <v>50.0</v>
       </c>
       <c r="D17" s="16">
@@ -8519,22 +9212,22 @@
       <c r="I17" s="16">
         <v>0.2913</v>
       </c>
-      <c r="J17" s="40">
+      <c r="J17" s="44">
         <v>-0.0013</v>
       </c>
-      <c r="K17" s="40">
+      <c r="K17" s="44">
         <v>0.41</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="21">
         <v>-0.0905</v>
       </c>
       <c r="M17" s="16">
         <v>0.3412</v>
       </c>
-      <c r="N17" s="40">
+      <c r="N17" s="44">
         <v>0.3277</v>
       </c>
-      <c r="O17" s="40">
+      <c r="O17" s="44">
         <v>2.1465</v>
       </c>
       <c r="P17" s="17">
@@ -8544,7 +9237,7 @@
     </row>
     <row r="18">
       <c r="B18" s="18"/>
-      <c r="C18" s="33">
+      <c r="C18" s="34">
         <v>75.0</v>
       </c>
       <c r="D18" s="16">
@@ -8565,22 +9258,22 @@
       <c r="I18" s="16">
         <v>0.4162</v>
       </c>
-      <c r="J18" s="40">
+      <c r="J18" s="44">
         <v>-0.0034</v>
       </c>
-      <c r="K18" s="40">
+      <c r="K18" s="44">
         <v>0.4013</v>
       </c>
-      <c r="L18" s="41">
+      <c r="L18" s="21">
         <v>-0.0952</v>
       </c>
       <c r="M18" s="16">
         <v>0.3118</v>
       </c>
-      <c r="N18" s="40">
+      <c r="N18" s="44">
         <v>0.3027</v>
       </c>
-      <c r="O18" s="40">
+      <c r="O18" s="44">
         <v>1.5061</v>
       </c>
       <c r="P18" s="17">
@@ -8590,7 +9283,7 @@
     </row>
     <row r="19">
       <c r="B19" s="9"/>
-      <c r="C19" s="34">
+      <c r="C19" s="35">
         <v>100.0</v>
       </c>
       <c r="D19" s="16">
@@ -8611,22 +9304,22 @@
       <c r="I19" s="16">
         <v>0.7157</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J19" s="44">
         <v>-0.0024</v>
       </c>
-      <c r="K19" s="40">
+      <c r="K19" s="44">
         <v>0.5579</v>
       </c>
-      <c r="L19" s="41">
+      <c r="L19" s="21">
         <v>-0.0783</v>
       </c>
       <c r="M19" s="16">
         <v>0.4064</v>
       </c>
-      <c r="N19" s="40">
+      <c r="N19" s="44">
         <v>0.3117</v>
       </c>
-      <c r="O19" s="40">
+      <c r="O19" s="44">
         <v>1.9388</v>
       </c>
       <c r="P19" s="17">
@@ -8635,10 +9328,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="36">
         <v>0.0</v>
       </c>
       <c r="D20" s="16">
@@ -8659,22 +9352,22 @@
       <c r="I20" s="16">
         <v>0.0</v>
       </c>
-      <c r="J20" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="K20" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="L20" s="40">
+      <c r="J20" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="44">
         <v>0.0</v>
       </c>
       <c r="M20" s="16">
         <v>0.0</v>
       </c>
-      <c r="N20" s="40">
-        <v>0.0</v>
-      </c>
-      <c r="O20" s="40">
+      <c r="N20" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="O20" s="44">
         <v>0.0</v>
       </c>
       <c r="P20" s="17">
@@ -8684,7 +9377,7 @@
     </row>
     <row r="21">
       <c r="B21" s="18"/>
-      <c r="C21" s="36">
+      <c r="C21" s="37">
         <v>25.0</v>
       </c>
       <c r="D21" s="16">
@@ -8705,22 +9398,22 @@
       <c r="I21" s="16">
         <v>0.2433</v>
       </c>
-      <c r="J21" s="40">
+      <c r="J21" s="44">
         <v>0.0013</v>
       </c>
-      <c r="K21" s="40">
+      <c r="K21" s="44">
         <v>0.2269</v>
       </c>
-      <c r="L21" s="41">
+      <c r="L21" s="21">
         <v>-0.1122</v>
       </c>
       <c r="M21" s="16">
         <v>0.2229</v>
       </c>
-      <c r="N21" s="40">
+      <c r="N21" s="44">
         <v>0.2716</v>
       </c>
-      <c r="O21" s="40">
+      <c r="O21" s="44">
         <v>0.4633</v>
       </c>
       <c r="P21" s="17">
@@ -8730,7 +9423,7 @@
     </row>
     <row r="22">
       <c r="B22" s="18"/>
-      <c r="C22" s="37">
+      <c r="C22" s="38">
         <v>50.0</v>
       </c>
       <c r="D22" s="16">
@@ -8751,22 +9444,22 @@
       <c r="I22" s="16">
         <v>0.2913</v>
       </c>
-      <c r="J22" s="40">
+      <c r="J22" s="44">
         <v>-0.0026</v>
       </c>
-      <c r="K22" s="40">
+      <c r="K22" s="44">
         <v>0.354</v>
       </c>
-      <c r="L22" s="41">
+      <c r="L22" s="21">
         <v>-0.0966</v>
       </c>
       <c r="M22" s="16">
         <v>0.3018</v>
       </c>
-      <c r="N22" s="40">
+      <c r="N22" s="44">
         <v>0.3151</v>
       </c>
-      <c r="O22" s="40">
+      <c r="O22" s="44">
         <v>1.4753</v>
       </c>
       <c r="P22" s="17">
@@ -8776,7 +9469,7 @@
     </row>
     <row r="23">
       <c r="B23" s="18"/>
-      <c r="C23" s="38">
+      <c r="C23" s="39">
         <v>75.0</v>
       </c>
       <c r="D23" s="16">
@@ -8797,22 +9490,22 @@
       <c r="I23" s="16">
         <v>0.4162</v>
       </c>
-      <c r="J23" s="40">
+      <c r="J23" s="44">
         <v>0.0043</v>
       </c>
-      <c r="K23" s="40">
+      <c r="K23" s="44">
         <v>0.446</v>
       </c>
-      <c r="L23" s="41">
+      <c r="L23" s="21">
         <v>-0.1063</v>
       </c>
       <c r="M23" s="16">
         <v>0.3849</v>
       </c>
-      <c r="N23" s="40">
+      <c r="N23" s="44">
         <v>0.3152</v>
       </c>
-      <c r="O23" s="40">
+      <c r="O23" s="44">
         <v>0.8311</v>
       </c>
       <c r="P23" s="17">
@@ -8822,7 +9515,7 @@
     </row>
     <row r="24">
       <c r="B24" s="9"/>
-      <c r="C24" s="39">
+      <c r="C24" s="40">
         <v>100.0</v>
       </c>
       <c r="D24" s="16">
@@ -8843,22 +9536,22 @@
       <c r="I24" s="16">
         <v>0.7157</v>
       </c>
-      <c r="J24" s="40">
+      <c r="J24" s="44">
         <v>0.0021</v>
       </c>
-      <c r="K24" s="40">
+      <c r="K24" s="44">
         <v>0.4587</v>
       </c>
-      <c r="L24" s="41">
+      <c r="L24" s="21">
         <v>-0.1033</v>
       </c>
       <c r="M24" s="16">
         <v>0.3439</v>
       </c>
-      <c r="N24" s="40">
+      <c r="N24" s="44">
         <v>0.272</v>
       </c>
-      <c r="O24" s="40">
+      <c r="O24" s="44">
         <v>0.7161</v>
       </c>
       <c r="P24" s="17">
@@ -11888,6 +12581,24 @@
       <c r="I5" s="16">
         <v>0.0</v>
       </c>
+      <c r="J5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N5" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O5" s="16">
+        <v>0.0</v>
+      </c>
       <c r="P5" s="17">
         <f t="shared" ref="P5:P24" si="1">I5-O5</f>
         <v>0</v>
@@ -11916,14 +12627,32 @@
       <c r="I6" s="16">
         <v>0.7161</v>
       </c>
+      <c r="J6" s="21">
+        <v>0.0172</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0.1803</v>
+      </c>
+      <c r="L6" s="16">
+        <v>-0.1151</v>
+      </c>
+      <c r="M6" s="21">
+        <v>0.0204</v>
+      </c>
+      <c r="N6" s="21">
+        <v>0.0607</v>
+      </c>
+      <c r="O6" s="21">
+        <v>0.164</v>
+      </c>
       <c r="P6" s="17">
         <f t="shared" si="1"/>
-        <v>0.7161</v>
+        <v>0.5521</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="18"/>
-      <c r="C7" s="21">
+      <c r="C7" s="22">
         <v>50.0</v>
       </c>
       <c r="D7" s="20">
@@ -11944,14 +12673,32 @@
       <c r="I7" s="16">
         <v>2.0249</v>
       </c>
+      <c r="J7" s="21">
+        <v>0.018</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0.1989</v>
+      </c>
+      <c r="L7" s="16">
+        <v>-0.1029</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0.0203</v>
+      </c>
+      <c r="N7" s="21">
+        <v>0.0545</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0.3636</v>
+      </c>
       <c r="P7" s="17">
         <f t="shared" si="1"/>
-        <v>2.0249</v>
+        <v>1.6613</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="18"/>
-      <c r="C8" s="22">
+      <c r="C8" s="23">
         <v>75.0</v>
       </c>
       <c r="D8" s="20">
@@ -11972,14 +12719,32 @@
       <c r="I8" s="16">
         <v>1.0198</v>
       </c>
+      <c r="J8" s="21">
+        <v>0.0174</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0.2342</v>
+      </c>
+      <c r="L8" s="16">
+        <v>-0.0971</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0.0423</v>
+      </c>
+      <c r="N8" s="21">
+        <v>0.0661</v>
+      </c>
+      <c r="O8" s="21">
+        <v>0.6018</v>
+      </c>
       <c r="P8" s="17">
         <f t="shared" si="1"/>
-        <v>1.0198</v>
+        <v>0.418</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="9"/>
-      <c r="C9" s="23">
+      <c r="C9" s="24">
         <v>100.0</v>
       </c>
       <c r="D9" s="20">
@@ -12000,16 +12765,34 @@
       <c r="I9" s="16">
         <v>1.6505</v>
       </c>
+      <c r="J9" s="21">
+        <v>0.019</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0.2595</v>
+      </c>
+      <c r="L9" s="16">
+        <v>-0.0956</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0.047</v>
+      </c>
+      <c r="N9" s="21">
+        <v>0.0456</v>
+      </c>
+      <c r="O9" s="21">
+        <v>0.4077</v>
+      </c>
       <c r="P9" s="17">
         <f t="shared" si="1"/>
-        <v>1.6505</v>
+        <v>1.2428</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="26">
         <v>0.0</v>
       </c>
       <c r="D10" s="16">
@@ -12028,6 +12811,24 @@
         <v>0.0</v>
       </c>
       <c r="I10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N10" s="21">
+        <v>0.0563</v>
+      </c>
+      <c r="O10" s="16">
         <v>0.0</v>
       </c>
       <c r="P10" s="17">
@@ -12037,7 +12838,7 @@
     </row>
     <row r="11">
       <c r="B11" s="18"/>
-      <c r="C11" s="26">
+      <c r="C11" s="27">
         <v>25.0</v>
       </c>
       <c r="D11" s="20">
@@ -12058,14 +12859,32 @@
       <c r="I11" s="16">
         <v>0.7161</v>
       </c>
+      <c r="J11" s="21">
+        <v>0.0184</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0.191</v>
+      </c>
+      <c r="L11" s="16">
+        <v>-0.1151</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0.0101</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O11" s="21">
+        <v>0.1723</v>
+      </c>
       <c r="P11" s="17">
         <f t="shared" si="1"/>
-        <v>0.7161</v>
+        <v>0.5438</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="18"/>
-      <c r="C12" s="27">
+      <c r="C12" s="28">
         <v>50.0</v>
       </c>
       <c r="D12" s="20">
@@ -12086,14 +12905,32 @@
       <c r="I12" s="16">
         <v>2.0249</v>
       </c>
+      <c r="J12" s="21">
+        <v>0.0178</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0.2359</v>
+      </c>
+      <c r="L12" s="16">
+        <v>-0.1029</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0.0255</v>
+      </c>
+      <c r="N12" s="21">
+        <v>0.074</v>
+      </c>
+      <c r="O12" s="21">
+        <v>0.4203</v>
+      </c>
       <c r="P12" s="17">
         <f t="shared" si="1"/>
-        <v>2.0249</v>
+        <v>1.6046</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="18"/>
-      <c r="C13" s="28">
+      <c r="C13" s="29">
         <v>75.0</v>
       </c>
       <c r="D13" s="20">
@@ -12114,14 +12951,32 @@
       <c r="I13" s="16">
         <v>1.0198</v>
       </c>
+      <c r="J13" s="21">
+        <v>0.0225</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0.268</v>
+      </c>
+      <c r="L13" s="16">
+        <v>-0.0971</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0.0493</v>
+      </c>
+      <c r="N13" s="21">
+        <v>0.0832</v>
+      </c>
+      <c r="O13" s="21">
+        <v>0.6428</v>
+      </c>
       <c r="P13" s="17">
         <f t="shared" si="1"/>
-        <v>1.0198</v>
+        <v>0.377</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="9"/>
-      <c r="C14" s="29">
+      <c r="C14" s="30">
         <v>100.0</v>
       </c>
       <c r="D14" s="20">
@@ -12142,16 +12997,34 @@
       <c r="I14" s="16">
         <v>1.6505</v>
       </c>
+      <c r="J14" s="21">
+        <v>0.0211</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0.2342</v>
+      </c>
+      <c r="L14" s="16">
+        <v>-0.0956</v>
+      </c>
+      <c r="M14" s="21">
+        <v>0.0332</v>
+      </c>
+      <c r="N14" s="21">
+        <v>0.0415</v>
+      </c>
+      <c r="O14" s="21">
+        <v>0.2664</v>
+      </c>
       <c r="P14" s="17">
         <f t="shared" si="1"/>
-        <v>1.6505</v>
+        <v>1.3841</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="31">
         <v>0.0</v>
       </c>
       <c r="D15" s="16">
@@ -12170,6 +13043,24 @@
         <v>0.0</v>
       </c>
       <c r="I15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="K15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N15" s="21">
+        <v>0.0719</v>
+      </c>
+      <c r="O15" s="16">
         <v>0.0</v>
       </c>
       <c r="P15" s="17">
@@ -12179,7 +13070,7 @@
     </row>
     <row r="16">
       <c r="B16" s="18"/>
-      <c r="C16" s="31">
+      <c r="C16" s="32">
         <v>25.0</v>
       </c>
       <c r="D16" s="20">
@@ -12200,14 +13091,32 @@
       <c r="I16" s="16">
         <v>0.6219</v>
       </c>
+      <c r="J16" s="21">
+        <v>0.0192</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0.1923</v>
+      </c>
+      <c r="L16" s="16">
+        <v>-0.1053</v>
+      </c>
+      <c r="M16" s="21">
+        <v>0.0188</v>
+      </c>
+      <c r="N16" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O16" s="21">
+        <v>0.1528</v>
+      </c>
       <c r="P16" s="17">
         <f t="shared" si="1"/>
-        <v>0.6219</v>
+        <v>0.4691</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="18"/>
-      <c r="C17" s="32">
+      <c r="C17" s="33">
         <v>50.0</v>
       </c>
       <c r="D17" s="20">
@@ -12228,14 +13137,32 @@
       <c r="I17" s="16">
         <v>0.688</v>
       </c>
+      <c r="J17" s="21">
+        <v>0.0205</v>
+      </c>
+      <c r="K17" s="21">
+        <v>0.2292</v>
+      </c>
+      <c r="L17" s="16">
+        <v>-0.1167</v>
+      </c>
+      <c r="M17" s="21">
+        <v>0.0368</v>
+      </c>
+      <c r="N17" s="21">
+        <v>0.0483</v>
+      </c>
+      <c r="O17" s="21">
+        <v>0.4713</v>
+      </c>
       <c r="P17" s="17">
         <f t="shared" si="1"/>
-        <v>0.688</v>
+        <v>0.2167</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="18"/>
-      <c r="C18" s="33">
+      <c r="C18" s="34">
         <v>75.0</v>
       </c>
       <c r="D18" s="20">
@@ -12256,14 +13183,32 @@
       <c r="I18" s="16">
         <v>0.8298</v>
       </c>
+      <c r="J18" s="21">
+        <v>0.0218</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0.2523</v>
+      </c>
+      <c r="L18" s="16">
+        <v>-0.1134</v>
+      </c>
+      <c r="M18" s="21">
+        <v>0.0331</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0.0534</v>
+      </c>
+      <c r="O18" s="21">
+        <v>0.5131</v>
+      </c>
       <c r="P18" s="17">
         <f t="shared" si="1"/>
-        <v>0.8298</v>
+        <v>0.3167</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="9"/>
-      <c r="C19" s="34">
+      <c r="C19" s="35">
         <v>100.0</v>
       </c>
       <c r="D19" s="20">
@@ -12284,16 +13229,34 @@
       <c r="I19" s="16">
         <v>0.7797</v>
       </c>
+      <c r="J19" s="21">
+        <v>0.0193</v>
+      </c>
+      <c r="K19" s="21">
+        <v>0.2414</v>
+      </c>
+      <c r="L19" s="16">
+        <v>0.1109</v>
+      </c>
+      <c r="M19" s="21">
+        <v>0.041</v>
+      </c>
+      <c r="N19" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="O19" s="21">
+        <v>0.4162</v>
+      </c>
       <c r="P19" s="17">
         <f t="shared" si="1"/>
-        <v>0.7797</v>
+        <v>0.3635</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="36">
         <v>0.0</v>
       </c>
       <c r="D20" s="16">
@@ -12312,6 +13275,24 @@
         <v>0.0</v>
       </c>
       <c r="I20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="J20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="M20" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="N20" s="21">
+        <v>0.0402</v>
+      </c>
+      <c r="O20" s="16">
         <v>0.0</v>
       </c>
       <c r="P20" s="17">
@@ -12321,7 +13302,7 @@
     </row>
     <row r="21">
       <c r="B21" s="18"/>
-      <c r="C21" s="36">
+      <c r="C21" s="37">
         <v>25.0</v>
       </c>
       <c r="D21" s="20">
@@ -12342,14 +13323,32 @@
       <c r="I21" s="16">
         <v>0.6219</v>
       </c>
+      <c r="J21" s="21">
+        <v>0.023</v>
+      </c>
+      <c r="K21" s="21">
+        <v>0.1857</v>
+      </c>
+      <c r="L21" s="16">
+        <v>-0.1053</v>
+      </c>
+      <c r="M21" s="21">
+        <v>0.0167</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="O21" s="21">
+        <v>0.3498</v>
+      </c>
       <c r="P21" s="17">
         <f t="shared" si="1"/>
-        <v>0.6219</v>
+        <v>0.2721</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="18"/>
-      <c r="C22" s="37">
+      <c r="C22" s="38">
         <v>50.0</v>
       </c>
       <c r="D22" s="20">
@@ -12370,14 +13369,32 @@
       <c r="I22" s="16">
         <v>0.688</v>
       </c>
+      <c r="J22" s="21">
+        <v>0.0255</v>
+      </c>
+      <c r="K22" s="21">
+        <v>0.2313</v>
+      </c>
+      <c r="L22" s="16">
+        <v>-0.1167</v>
+      </c>
+      <c r="M22" s="21">
+        <v>0.0403</v>
+      </c>
+      <c r="N22" s="21">
+        <v>0.0767</v>
+      </c>
+      <c r="O22" s="21">
+        <v>0.3921</v>
+      </c>
       <c r="P22" s="17">
         <f t="shared" si="1"/>
-        <v>0.688</v>
+        <v>0.2959</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="18"/>
-      <c r="C23" s="38">
+      <c r="C23" s="39">
         <v>75.0</v>
       </c>
       <c r="D23" s="20">
@@ -12398,14 +13415,32 @@
       <c r="I23" s="16">
         <v>0.8298</v>
       </c>
+      <c r="J23" s="21">
+        <v>0.0227</v>
+      </c>
+      <c r="K23" s="21">
+        <v>0.2571</v>
+      </c>
+      <c r="L23" s="16">
+        <v>-0.1134</v>
+      </c>
+      <c r="M23" s="21">
+        <v>0.0484</v>
+      </c>
+      <c r="N23" s="21">
+        <v>0.0515</v>
+      </c>
+      <c r="O23" s="21">
+        <v>0.3853</v>
+      </c>
       <c r="P23" s="17">
         <f t="shared" si="1"/>
-        <v>0.8298</v>
+        <v>0.4445</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="9"/>
-      <c r="C24" s="39">
+      <c r="C24" s="40">
         <v>100.0</v>
       </c>
       <c r="D24" s="20">
@@ -12426,9 +13461,27 @@
       <c r="I24" s="16">
         <v>0.7797</v>
       </c>
+      <c r="J24" s="21">
+        <v>0.0258</v>
+      </c>
+      <c r="K24" s="21">
+        <v>0.2645</v>
+      </c>
+      <c r="L24" s="16">
+        <v>0.1109</v>
+      </c>
+      <c r="M24" s="21">
+        <v>0.0682</v>
+      </c>
+      <c r="N24" s="21">
+        <v>0.0695</v>
+      </c>
+      <c r="O24" s="21">
+        <v>0.7124</v>
+      </c>
       <c r="P24" s="17">
         <f t="shared" si="1"/>
-        <v>0.7797</v>
+        <v>0.0673</v>
       </c>
     </row>
     <row r="25">

</xml_diff>